<commit_message>
HuyenPT: Commit source code for Admin_Slider
+ Source mapping with UI
+ MongoDB
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/List of UseCase.xlsx
+++ b/WIP/Users/HuyenPT/List of UseCase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="222">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -679,6 +679,9 @@
   </si>
   <si>
     <t>Send mail</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -850,7 +853,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -897,32 +900,59 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -936,12 +966,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -951,32 +981,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1279,12 +1288,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D5:G82"/>
+  <dimension ref="C5:G82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F82" sqref="F82"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="9" style="43"/>
     <col min="4" max="4" width="10.75" style="2" customWidth="1"/>
     <col min="5" max="5" width="19.625" style="2" customWidth="1"/>
     <col min="6" max="6" width="28.625" style="3" bestFit="1" customWidth="1"/>
@@ -1292,7 +1304,7 @@
     <col min="8" max="8" width="15.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:7" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:7" ht="28.5" x14ac:dyDescent="0.25">
       <c r="D5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,27 +1318,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="23" t="s">
+    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D6" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-    </row>
-    <row r="7" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="34" t="s">
+      <c r="E6" s="26"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+    </row>
+    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D7" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="34"/>
-      <c r="G7" s="34"/>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="18" t="s">
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+    </row>
+    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D8" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="18" t="s">
+      <c r="E8" s="28" t="s">
         <v>198</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1336,9 +1348,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D9" s="29"/>
+      <c r="E9" s="29"/>
       <c r="F9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1346,9 +1358,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="19"/>
-      <c r="E10" s="24"/>
+    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="D10" s="30"/>
+      <c r="E10" s="29"/>
       <c r="F10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1356,11 +1371,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="19"/>
+      <c r="E11" s="30"/>
       <c r="F11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1368,11 +1383,14 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D12" s="18" t="s">
+    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="43" t="s">
+        <v>221</v>
+      </c>
+      <c r="D12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="18" t="s">
+      <c r="E12" s="28" t="s">
         <v>17</v>
       </c>
       <c r="F12" s="4" t="s">
@@ -1382,9 +1400,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D13" s="19"/>
-      <c r="E13" s="19"/>
+    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="44">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="4" t="s">
         <v>131</v>
       </c>
@@ -1392,7 +1413,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D14" s="5" t="s">
         <v>20</v>
       </c>
@@ -1404,7 +1425,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D15" s="5" t="s">
         <v>22</v>
       </c>
@@ -1416,19 +1437,19 @@
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="35" t="s">
+    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D16" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="36"/>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="33"/>
     </row>
     <row r="17" spans="4:7" ht="45" x14ac:dyDescent="0.25">
       <c r="D17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="18" t="s">
+      <c r="E17" s="28" t="s">
         <v>47</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1439,10 +1460,10 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="18" t="s">
+      <c r="D18" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="24"/>
+      <c r="E18" s="29"/>
       <c r="F18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1451,8 +1472,8 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="19"/>
-      <c r="E19" s="24"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="29"/>
       <c r="F19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1464,7 +1485,7 @@
       <c r="D20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="24"/>
+      <c r="E20" s="29"/>
       <c r="F20" s="4" t="s">
         <v>31</v>
       </c>
@@ -1476,7 +1497,7 @@
       <c r="D21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="24"/>
+      <c r="E21" s="29"/>
       <c r="F21" s="4" t="s">
         <v>53</v>
       </c>
@@ -1488,7 +1509,7 @@
       <c r="D22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="19"/>
+      <c r="E22" s="30"/>
       <c r="F22" s="4" t="s">
         <v>54</v>
       </c>
@@ -1500,7 +1521,7 @@
       <c r="D23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="18" t="s">
+      <c r="E23" s="28" t="s">
         <v>48</v>
       </c>
       <c r="F23" s="4" t="s">
@@ -1514,7 +1535,7 @@
       <c r="D24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="24"/>
+      <c r="E24" s="29"/>
       <c r="F24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1526,7 +1547,7 @@
       <c r="D25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="24"/>
+      <c r="E25" s="29"/>
       <c r="F25" s="4" t="s">
         <v>43</v>
       </c>
@@ -1538,7 +1559,7 @@
       <c r="D26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="19"/>
+      <c r="E26" s="30"/>
       <c r="F26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1550,7 +1571,7 @@
       <c r="D27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="28" t="s">
+      <c r="E27" s="37" t="s">
         <v>46</v>
       </c>
       <c r="F27" s="4" t="s">
@@ -1564,7 +1585,7 @@
       <c r="D28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="30"/>
+      <c r="E28" s="38"/>
       <c r="F28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1576,7 +1597,7 @@
       <c r="D29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="30"/>
+      <c r="E29" s="38"/>
       <c r="F29" s="4" t="s">
         <v>45</v>
       </c>
@@ -1588,7 +1609,7 @@
       <c r="D30" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="29"/>
+      <c r="E30" s="39"/>
       <c r="F30" s="4" t="s">
         <v>35</v>
       </c>
@@ -1597,18 +1618,18 @@
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="32"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
+      <c r="G31" s="42"/>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="28" t="s">
+      <c r="E32" s="37" t="s">
         <v>199</v>
       </c>
       <c r="F32" s="4" t="s">
@@ -1622,7 +1643,7 @@
       <c r="D33" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="30"/>
+      <c r="E33" s="38"/>
       <c r="F33" s="6" t="s">
         <v>69</v>
       </c>
@@ -1634,7 +1655,7 @@
       <c r="D34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="29"/>
+      <c r="E34" s="39"/>
       <c r="F34" s="6" t="s">
         <v>115</v>
       </c>
@@ -1646,7 +1667,7 @@
       <c r="D35" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="28" t="s">
         <v>200</v>
       </c>
       <c r="F35" s="4" t="s">
@@ -1660,7 +1681,7 @@
       <c r="D36" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="24"/>
+      <c r="E36" s="29"/>
       <c r="F36" s="4" t="s">
         <v>100</v>
       </c>
@@ -1672,7 +1693,7 @@
       <c r="D37" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="19"/>
+      <c r="E37" s="30"/>
       <c r="F37" s="4" t="s">
         <v>116</v>
       </c>
@@ -1681,18 +1702,18 @@
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="25" t="s">
+      <c r="D38" s="34" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="26"/>
-      <c r="F38" s="26"/>
-      <c r="G38" s="27"/>
+      <c r="E38" s="35"/>
+      <c r="F38" s="35"/>
+      <c r="G38" s="36"/>
     </row>
     <row r="39" spans="4:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D39" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E39" s="18" t="s">
+      <c r="E39" s="28" t="s">
         <v>201</v>
       </c>
       <c r="F39" s="4" t="s">
@@ -1706,7 +1727,7 @@
       <c r="D40" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="24"/>
+      <c r="E40" s="29"/>
       <c r="F40" s="4" t="s">
         <v>84</v>
       </c>
@@ -1718,7 +1739,7 @@
       <c r="D41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="19"/>
+      <c r="E41" s="30"/>
       <c r="F41" s="4" t="s">
         <v>88</v>
       </c>
@@ -1730,7 +1751,7 @@
       <c r="D42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E42" s="28" t="s">
+      <c r="E42" s="37" t="s">
         <v>119</v>
       </c>
       <c r="F42" s="6" t="s">
@@ -1744,7 +1765,7 @@
       <c r="D43" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="30"/>
+      <c r="E43" s="38"/>
       <c r="F43" s="6" t="s">
         <v>76</v>
       </c>
@@ -1756,7 +1777,7 @@
       <c r="D44" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E44" s="30"/>
+      <c r="E44" s="38"/>
       <c r="F44" s="4" t="s">
         <v>77</v>
       </c>
@@ -1768,7 +1789,7 @@
       <c r="D45" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E45" s="29"/>
+      <c r="E45" s="39"/>
       <c r="F45" s="4" t="s">
         <v>82</v>
       </c>
@@ -1780,7 +1801,7 @@
       <c r="D46" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E46" s="28" t="s">
         <v>90</v>
       </c>
       <c r="F46" s="8" t="s">
@@ -1794,7 +1815,7 @@
       <c r="D47" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E47" s="24"/>
+      <c r="E47" s="29"/>
       <c r="F47" s="4" t="s">
         <v>91</v>
       </c>
@@ -1806,7 +1827,7 @@
       <c r="D48" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E48" s="19"/>
+      <c r="E48" s="30"/>
       <c r="F48" s="4" t="s">
         <v>92</v>
       </c>
@@ -1814,15 +1835,15 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="25" t="s">
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D49" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="E49" s="26"/>
-      <c r="F49" s="26"/>
-      <c r="G49" s="27"/>
-    </row>
-    <row r="50" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E49" s="35"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="36"/>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D50" s="5" t="s">
         <v>149</v>
       </c>
@@ -1834,7 +1855,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D51" s="5" t="s">
         <v>150</v>
       </c>
@@ -1846,19 +1867,19 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D52" s="23" t="s">
+    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D52" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="E52" s="23"/>
-      <c r="F52" s="23"/>
-      <c r="G52" s="23"/>
-    </row>
-    <row r="53" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E52" s="26"/>
+      <c r="F52" s="26"/>
+      <c r="G52" s="26"/>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D53" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E53" s="20" t="s">
+      <c r="E53" s="17" t="s">
         <v>123</v>
       </c>
       <c r="F53" s="10" t="s">
@@ -1866,11 +1887,11 @@
       </c>
       <c r="G53" s="10"/>
     </row>
-    <row r="54" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D54" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E54" s="21"/>
+      <c r="E54" s="18"/>
       <c r="F54" s="10" t="s">
         <v>125</v>
       </c>
@@ -1878,11 +1899,11 @@
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D55" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E55" s="21"/>
+      <c r="E55" s="18"/>
       <c r="F55" s="10" t="s">
         <v>126</v>
       </c>
@@ -1890,11 +1911,11 @@
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D56" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E56" s="21"/>
+      <c r="E56" s="18"/>
       <c r="F56" s="10" t="s">
         <v>129</v>
       </c>
@@ -1902,11 +1923,11 @@
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D57" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="21"/>
+      <c r="E57" s="18"/>
       <c r="F57" s="11" t="s">
         <v>183</v>
       </c>
@@ -1914,11 +1935,11 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D58" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E58" s="22"/>
+      <c r="E58" s="19"/>
       <c r="F58" s="11" t="s">
         <v>184</v>
       </c>
@@ -1926,11 +1947,14 @@
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C59" s="43" t="s">
+        <v>221</v>
+      </c>
       <c r="D59" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="E59" s="20" t="s">
+      <c r="E59" s="17" t="s">
         <v>137</v>
       </c>
       <c r="F59" s="10" t="s">
@@ -1940,11 +1964,14 @@
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C60" s="43" t="s">
+        <v>221</v>
+      </c>
       <c r="D60" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E60" s="21"/>
+      <c r="E60" s="18"/>
       <c r="F60" s="10" t="s">
         <v>139</v>
       </c>
@@ -1952,11 +1979,11 @@
         <v>142</v>
       </c>
     </row>
-    <row r="61" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D61" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E61" s="22"/>
+      <c r="E61" s="19"/>
       <c r="F61" s="11" t="s">
         <v>140</v>
       </c>
@@ -1964,11 +1991,14 @@
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C62" s="44" t="s">
+        <v>221</v>
+      </c>
       <c r="D62" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E62" s="20" t="s">
+      <c r="E62" s="17" t="s">
         <v>144</v>
       </c>
       <c r="F62" s="10" t="s">
@@ -1978,11 +2008,14 @@
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C63" s="43" t="s">
+        <v>221</v>
+      </c>
       <c r="D63" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E63" s="21"/>
+      <c r="E63" s="18"/>
       <c r="F63" s="10" t="s">
         <v>145</v>
       </c>
@@ -1990,11 +2023,11 @@
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
       <c r="D64" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E64" s="22"/>
+      <c r="E64" s="19"/>
       <c r="F64" s="10" t="s">
         <v>146</v>
       </c>
@@ -2002,11 +2035,14 @@
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65" s="43" t="s">
+        <v>221</v>
+      </c>
       <c r="D65" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E65" s="20" t="s">
+      <c r="E65" s="17" t="s">
         <v>191</v>
       </c>
       <c r="F65" s="10" t="s">
@@ -2016,11 +2052,14 @@
         <v>170</v>
       </c>
     </row>
-    <row r="66" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C66" s="43" t="s">
+        <v>221</v>
+      </c>
       <c r="D66" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E66" s="21"/>
+      <c r="E66" s="18"/>
       <c r="F66" s="10" t="s">
         <v>193</v>
       </c>
@@ -2028,11 +2067,14 @@
         <v>171</v>
       </c>
     </row>
-    <row r="67" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C67" s="43" t="s">
+        <v>221</v>
+      </c>
       <c r="D67" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="E67" s="22"/>
+      <c r="E67" s="19"/>
       <c r="F67" s="10" t="s">
         <v>194</v>
       </c>
@@ -2040,11 +2082,11 @@
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D68" s="20" t="s">
+    <row r="68" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D68" s="17" t="s">
         <v>179</v>
       </c>
-      <c r="E68" s="20" t="s">
+      <c r="E68" s="17" t="s">
         <v>163</v>
       </c>
       <c r="F68" s="11" t="s">
@@ -2054,9 +2096,9 @@
         <v>206</v>
       </c>
     </row>
-    <row r="69" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D69" s="21"/>
-      <c r="E69" s="21"/>
+    <row r="69" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D69" s="18"/>
+      <c r="E69" s="18"/>
       <c r="F69" s="11" t="s">
         <v>202</v>
       </c>
@@ -2064,9 +2106,9 @@
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D70" s="21"/>
-      <c r="E70" s="21"/>
+    <row r="70" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="D70" s="18"/>
+      <c r="E70" s="18"/>
       <c r="F70" s="11" t="s">
         <v>204</v>
       </c>
@@ -2074,9 +2116,9 @@
         <v>208</v>
       </c>
     </row>
-    <row r="71" spans="4:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="D71" s="21"/>
-      <c r="E71" s="21"/>
+    <row r="71" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="D71" s="18"/>
+      <c r="E71" s="18"/>
       <c r="F71" s="11" t="s">
         <v>205</v>
       </c>
@@ -2084,9 +2126,9 @@
         <v>209</v>
       </c>
     </row>
-    <row r="72" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D72" s="22"/>
-      <c r="E72" s="22"/>
+    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D72" s="19"/>
+      <c r="E72" s="19"/>
       <c r="F72" s="11" t="s">
         <v>164</v>
       </c>
@@ -2094,19 +2136,19 @@
         <v>210</v>
       </c>
     </row>
-    <row r="73" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D73" s="23" t="s">
+    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D73" s="26" t="s">
         <v>173</v>
       </c>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-    </row>
-    <row r="74" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D74" s="42" t="s">
+      <c r="E73" s="26"/>
+      <c r="F73" s="26"/>
+      <c r="G73" s="26"/>
+    </row>
+    <row r="74" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D74" s="23" t="s">
         <v>180</v>
       </c>
-      <c r="E74" s="16" t="s">
+      <c r="E74" s="20" t="s">
         <v>220</v>
       </c>
       <c r="F74" s="14" t="s">
@@ -2116,9 +2158,9 @@
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D75" s="40"/>
-      <c r="E75" s="39"/>
+    <row r="75" spans="3:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="D75" s="24"/>
+      <c r="E75" s="21"/>
       <c r="F75" s="14" t="s">
         <v>195</v>
       </c>
@@ -2126,9 +2168,9 @@
         <v>176</v>
       </c>
     </row>
-    <row r="76" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="41"/>
-      <c r="E76" s="17"/>
+    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D76" s="25"/>
+      <c r="E76" s="22"/>
       <c r="F76" s="14" t="s">
         <v>186</v>
       </c>
@@ -2136,44 +2178,44 @@
         <v>189</v>
       </c>
     </row>
-    <row r="77" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D77" s="16" t="s">
+    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D77" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="E77" s="16" t="s">
+      <c r="E77" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="F77" s="38" t="s">
+      <c r="F77" s="16" t="s">
         <v>211</v>
       </c>
       <c r="G77" s="14" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="78" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="38" t="s">
+    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D78" s="21"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="16" t="s">
         <v>212</v>
       </c>
       <c r="G78" s="13" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="79" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="39"/>
-      <c r="E79" s="39"/>
-      <c r="F79" s="38" t="s">
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D79" s="21"/>
+      <c r="E79" s="21"/>
+      <c r="F79" s="16" t="s">
         <v>213</v>
       </c>
       <c r="G79" s="13" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="80" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
-      <c r="F80" s="38" t="s">
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="D80" s="21"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="16" t="s">
         <v>214</v>
       </c>
       <c r="G80" s="13" t="s">
@@ -2181,9 +2223,9 @@
       </c>
     </row>
     <row r="81" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D81" s="17"/>
-      <c r="E81" s="17"/>
-      <c r="F81" s="38" t="s">
+      <c r="D81" s="22"/>
+      <c r="E81" s="22"/>
+      <c r="F81" s="16" t="s">
         <v>181</v>
       </c>
       <c r="G81" s="13" t="s">
@@ -2204,37 +2246,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="D68:D72"/>
-    <mergeCell ref="E77:E81"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="E68:E72"/>
+    <mergeCell ref="D73:G73"/>
+    <mergeCell ref="D52:G52"/>
+    <mergeCell ref="E53:E58"/>
+    <mergeCell ref="E42:E45"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E59:E61"/>
+    <mergeCell ref="E62:E64"/>
+    <mergeCell ref="E46:E48"/>
+    <mergeCell ref="D49:G49"/>
+    <mergeCell ref="E27:E30"/>
+    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D38:G38"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E17:E22"/>
+    <mergeCell ref="E23:E26"/>
+    <mergeCell ref="E32:E34"/>
+    <mergeCell ref="E35:E37"/>
     <mergeCell ref="D6:G6"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="D8:D10"/>
     <mergeCell ref="D16:G16"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="E8:E11"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="E68:E72"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="E53:E58"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="D31:G31"/>
+    <mergeCell ref="D68:D72"/>
+    <mergeCell ref="E77:E81"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="E74:E76"/>
+    <mergeCell ref="D74:D76"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Document]_Commit file tracking tiến độ dự án
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/List of UseCase.xlsx
+++ b/WIP/Users/HuyenPT/List of UseCase.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="90" windowWidth="20115" windowHeight="7500"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -679,9 +679,6 @@
   </si>
   <si>
     <t>Send mail</t>
-  </si>
-  <si>
-    <t>done</t>
   </si>
 </sst>
 </file>
@@ -853,7 +850,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -912,6 +909,57 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -929,63 +977,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1288,995 +1279,962 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:G82"/>
+  <dimension ref="C5:F82"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F82" sqref="F82"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9" style="43"/>
-    <col min="4" max="4" width="10.75" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="28.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="40.75" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.375" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="40.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:7" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:6" ht="28.5" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="D5" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D6" s="26" t="s">
+    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C6" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D7" s="27" t="s">
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D8" s="28" t="s">
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
+      <c r="F7" s="33"/>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="28" t="s">
+      <c r="D8" s="24" t="s">
         <v>198</v>
       </c>
+      <c r="E8" s="4" t="s">
+        <v>6</v>
+      </c>
       <c r="F8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G8" s="4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D9" s="29"/>
-      <c r="E9" s="29"/>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="F9" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G9" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D10" s="30"/>
-      <c r="E10" s="29"/>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="26"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="F10" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G10" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D11" s="5" t="s">
+    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E11" s="30"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="4" t="s">
+        <v>13</v>
+      </c>
       <c r="F11" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D12" s="28" t="s">
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="28" t="s">
+      <c r="D12" s="24" t="s">
         <v>17</v>
       </c>
+      <c r="E12" s="4" t="s">
+        <v>132</v>
+      </c>
       <c r="F12" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="G12" s="4" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="44">
-        <v>0.5</v>
-      </c>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="4" t="s">
+        <v>131</v>
+      </c>
       <c r="F13" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="G13" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D14" s="5" t="s">
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="4" t="s">
+        <v>18</v>
+      </c>
       <c r="F14" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D15" s="5" t="s">
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="4" t="s">
+        <v>196</v>
+      </c>
       <c r="F15" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="G15" s="4" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D16" s="31" t="s">
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33"/>
-    </row>
-    <row r="17" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D17" s="5" t="s">
+      <c r="D16" s="35"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="36"/>
+    </row>
+    <row r="17" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C17" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="28" t="s">
+      <c r="D17" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="4" t="s">
+      <c r="E17" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="6" t="s">
+      <c r="F17" s="6" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D18" s="28" t="s">
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="29"/>
+      <c r="D18" s="25"/>
+      <c r="E18" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="F18" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G18" s="4" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D19" s="30"/>
-      <c r="E19" s="29"/>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="26"/>
+      <c r="D19" s="25"/>
+      <c r="E19" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="F19" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D20" s="5" t="s">
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="29"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="F20" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D21" s="5" t="s">
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E21" s="29"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="4" t="s">
+        <v>53</v>
+      </c>
       <c r="F21" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D22" s="5" t="s">
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="30"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="4" t="s">
+        <v>54</v>
+      </c>
       <c r="F22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G22" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D23" s="5" t="s">
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="28" t="s">
+      <c r="D23" s="24" t="s">
         <v>48</v>
       </c>
+      <c r="E23" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="F23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="G23" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="5" t="s">
+    <row r="24" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C24" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="29"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="4" t="s">
+        <v>42</v>
+      </c>
       <c r="F24" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D25" s="5" t="s">
+    <row r="25" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C25" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="29"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="4" t="s">
+        <v>43</v>
+      </c>
       <c r="F25" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G25" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D26" s="5" t="s">
+    <row r="26" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C26" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="30"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="F26" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D27" s="5" t="s">
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C27" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="37" t="s">
+      <c r="D27" s="21" t="s">
         <v>46</v>
       </c>
+      <c r="E27" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="F27" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G27" s="4" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D28" s="5" t="s">
+    <row r="28" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C28" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="E28" s="38"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="4" t="s">
+        <v>44</v>
+      </c>
       <c r="F28" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G28" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D29" s="5" t="s">
+    <row r="29" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C29" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="E29" s="38"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="F29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="G29" s="4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D30" s="5" t="s">
+    <row r="30" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C30" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="E30" s="39"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="4" t="s">
+        <v>35</v>
+      </c>
       <c r="F30" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="G30" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D31" s="40" t="s">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C31" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="42"/>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D32" s="15" t="s">
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="32"/>
+    </row>
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E32" s="37" t="s">
+      <c r="D32" s="21" t="s">
         <v>199</v>
       </c>
+      <c r="E32" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="F32" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="G32" s="4" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D33" s="15" t="s">
+    <row r="33" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C33" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E33" s="38"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="F33" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G33" s="6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D34" s="15" t="s">
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C34" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="E34" s="39"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="6" t="s">
+        <v>115</v>
+      </c>
       <c r="F34" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="G34" s="6" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D35" s="15" t="s">
+    <row r="35" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C35" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="D35" s="24" t="s">
         <v>200</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="E35" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G35" s="6" t="s">
+      <c r="F35" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D36" s="15" t="s">
+    <row r="36" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C36" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E36" s="29"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="4" t="s">
+        <v>100</v>
+      </c>
       <c r="F36" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="G36" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D37" s="15" t="s">
+    <row r="37" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C37" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="30"/>
+      <c r="D37" s="26"/>
+      <c r="E37" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="F37" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G37" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D38" s="34" t="s">
+    <row r="38" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C38" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="E38" s="35"/>
-      <c r="F38" s="35"/>
-      <c r="G38" s="36"/>
-    </row>
-    <row r="39" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D39" s="5" t="s">
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="29"/>
+    </row>
+    <row r="39" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C39" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="E39" s="28" t="s">
+      <c r="D39" s="24" t="s">
         <v>201</v>
       </c>
-      <c r="F39" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="G39" s="6" t="s">
+      <c r="F39" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D40" s="5" t="s">
+    <row r="40" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C40" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="29"/>
-      <c r="F40" s="4" t="s">
+      <c r="D40" s="25"/>
+      <c r="E40" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="G40" s="6" t="s">
+      <c r="F40" s="6" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="41" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D41" s="5" t="s">
+    <row r="41" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C41" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="4" t="s">
+      <c r="D41" s="26"/>
+      <c r="E41" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="G41" s="6" t="s">
+      <c r="F41" s="6" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="42" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D42" s="5" t="s">
+    <row r="42" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C42" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="E42" s="37" t="s">
+      <c r="D42" s="21" t="s">
         <v>119</v>
       </c>
+      <c r="E42" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="F42" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G42" s="6" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D43" s="5" t="s">
+    <row r="43" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C43" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="E43" s="38"/>
-      <c r="F43" s="6" t="s">
+      <c r="D43" s="22"/>
+      <c r="E43" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="G43" s="7" t="s">
+      <c r="F43" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D44" s="5" t="s">
+    <row r="44" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C44" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="E44" s="38"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="4" t="s">
+        <v>77</v>
+      </c>
       <c r="F44" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="G44" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D45" s="5" t="s">
+    <row r="45" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C45" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="E45" s="39"/>
+      <c r="D45" s="23"/>
+      <c r="E45" s="4" t="s">
+        <v>82</v>
+      </c>
       <c r="F45" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="G45" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="46" spans="4:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D46" s="5" t="s">
+    <row r="46" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C46" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="E46" s="28" t="s">
+      <c r="D46" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="F46" s="8" t="s">
+      <c r="E46" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="F46" s="6" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D47" s="5" t="s">
+    <row r="47" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C47" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E47" s="29"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="4" t="s">
+        <v>91</v>
+      </c>
       <c r="F47" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="G47" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="48" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D48" s="5" t="s">
+    <row r="48" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C48" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="E48" s="30"/>
+      <c r="D48" s="26"/>
+      <c r="E48" s="4" t="s">
+        <v>92</v>
+      </c>
       <c r="F48" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="G48" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D49" s="34" t="s">
+    <row r="49" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C49" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="E49" s="35"/>
-      <c r="F49" s="35"/>
-      <c r="G49" s="36"/>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D50" s="5" t="s">
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="29"/>
+    </row>
+    <row r="50" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C50" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="E50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="4" t="s">
+        <v>110</v>
+      </c>
       <c r="F50" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="G50" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D51" s="5" t="s">
+    <row r="51" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C51" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="6" t="s">
+      <c r="D51" s="5"/>
+      <c r="E51" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="G51" s="4" t="s">
+      <c r="F51" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D52" s="26" t="s">
+    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C52" s="20" t="s">
         <v>114</v>
       </c>
-      <c r="E52" s="26"/>
-      <c r="F52" s="26"/>
-      <c r="G52" s="26"/>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D53" s="9" t="s">
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
+      <c r="F52" s="20"/>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="E53" s="17" t="s">
+      <c r="D53" s="17" t="s">
         <v>123</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="E53" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="G53" s="10"/>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D54" s="9" t="s">
+      <c r="F53" s="10"/>
+    </row>
+    <row r="54" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C54" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="E54" s="18"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="10" t="s">
+        <v>125</v>
+      </c>
       <c r="F54" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="G54" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D55" s="9" t="s">
+    <row r="55" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C55" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="E55" s="18"/>
+      <c r="D55" s="18"/>
+      <c r="E55" s="10" t="s">
+        <v>126</v>
+      </c>
       <c r="F55" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="G55" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D56" s="9" t="s">
+    <row r="56" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C56" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="E56" s="18"/>
+      <c r="D56" s="18"/>
+      <c r="E56" s="10" t="s">
+        <v>129</v>
+      </c>
       <c r="F56" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="G56" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="57" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D57" s="9" t="s">
+    <row r="57" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C57" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="E57" s="18"/>
-      <c r="F57" s="11" t="s">
+      <c r="D57" s="18"/>
+      <c r="E57" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="G57" s="10" t="s">
+      <c r="F57" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D58" s="9" t="s">
+    <row r="58" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C58" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="E58" s="19"/>
+      <c r="D58" s="19"/>
+      <c r="E58" s="11" t="s">
+        <v>184</v>
+      </c>
       <c r="F58" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="G58" s="11" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C59" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D59" s="9" t="s">
+    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C59" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="E59" s="17" t="s">
+      <c r="D59" s="17" t="s">
         <v>137</v>
       </c>
+      <c r="E59" s="10" t="s">
+        <v>138</v>
+      </c>
       <c r="F59" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="G59" s="10" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C60" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D60" s="9" t="s">
+    <row r="60" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C60" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="E60" s="18"/>
+      <c r="D60" s="18"/>
+      <c r="E60" s="10" t="s">
+        <v>139</v>
+      </c>
       <c r="F60" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="G60" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="61" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D61" s="9" t="s">
+    <row r="61" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C61" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="E61" s="19"/>
-      <c r="F61" s="11" t="s">
+      <c r="D61" s="19"/>
+      <c r="E61" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="G61" s="10" t="s">
+      <c r="F61" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C62" s="44" t="s">
-        <v>221</v>
-      </c>
-      <c r="D62" s="9" t="s">
+    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C62" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="E62" s="17" t="s">
+      <c r="D62" s="17" t="s">
         <v>144</v>
       </c>
+      <c r="E62" s="10" t="s">
+        <v>162</v>
+      </c>
       <c r="F62" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="G62" s="10" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C63" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D63" s="9" t="s">
+    <row r="63" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C63" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="E63" s="18"/>
+      <c r="D63" s="18"/>
+      <c r="E63" s="10" t="s">
+        <v>145</v>
+      </c>
       <c r="F63" s="10" t="s">
-        <v>145</v>
-      </c>
-      <c r="G63" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D64" s="9" t="s">
+    <row r="64" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C64" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="E64" s="19"/>
+      <c r="D64" s="19"/>
+      <c r="E64" s="10" t="s">
+        <v>146</v>
+      </c>
       <c r="F64" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="G64" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C65" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D65" s="9" t="s">
+    <row r="65" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C65" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="E65" s="17" t="s">
+      <c r="D65" s="17" t="s">
         <v>191</v>
       </c>
+      <c r="E65" s="10" t="s">
+        <v>192</v>
+      </c>
       <c r="F65" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="G65" s="10" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C66" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D66" s="9" t="s">
+    <row r="66" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C66" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="E66" s="18"/>
+      <c r="D66" s="18"/>
+      <c r="E66" s="10" t="s">
+        <v>193</v>
+      </c>
       <c r="F66" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="G66" s="10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C67" s="43" t="s">
-        <v>221</v>
-      </c>
-      <c r="D67" s="9" t="s">
+    <row r="67" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C67" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="E67" s="19"/>
+      <c r="D67" s="19"/>
+      <c r="E67" s="10" t="s">
+        <v>194</v>
+      </c>
       <c r="F67" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="G67" s="10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="68" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="68" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C68" s="17" t="s">
+        <v>179</v>
+      </c>
       <c r="D68" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="E68" s="17" t="s">
         <v>163</v>
       </c>
+      <c r="E68" s="11" t="s">
+        <v>203</v>
+      </c>
       <c r="F68" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="G68" s="11" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="69" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="69" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C69" s="18"/>
       <c r="D69" s="18"/>
-      <c r="E69" s="18"/>
+      <c r="E69" s="11" t="s">
+        <v>202</v>
+      </c>
       <c r="F69" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="G69" s="11" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="70" spans="3:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C70" s="18"/>
       <c r="D70" s="18"/>
-      <c r="E70" s="18"/>
+      <c r="E70" s="11" t="s">
+        <v>204</v>
+      </c>
       <c r="F70" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="G70" s="11" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="71" spans="3:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="71" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C71" s="18"/>
       <c r="D71" s="18"/>
-      <c r="E71" s="18"/>
+      <c r="E71" s="11" t="s">
+        <v>205</v>
+      </c>
       <c r="F71" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="G71" s="11" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="72" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C72" s="19"/>
       <c r="D72" s="19"/>
-      <c r="E72" s="19"/>
-      <c r="F72" s="11" t="s">
+      <c r="E72" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="G72" s="10" t="s">
+      <c r="F72" s="10" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="73" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D73" s="26" t="s">
+    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C73" s="20" t="s">
         <v>173</v>
       </c>
-      <c r="E73" s="26"/>
-      <c r="F73" s="26"/>
-      <c r="G73" s="26"/>
-    </row>
-    <row r="74" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D74" s="23" t="s">
+      <c r="D73" s="20"/>
+      <c r="E73" s="20"/>
+      <c r="F73" s="20"/>
+    </row>
+    <row r="74" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C74" s="40" t="s">
         <v>180</v>
       </c>
-      <c r="E74" s="20" t="s">
+      <c r="D74" s="37" t="s">
         <v>220</v>
       </c>
+      <c r="E74" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="F74" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="G74" s="14" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="75" spans="3:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="D75" s="24"/>
-      <c r="E75" s="21"/>
+    <row r="75" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C75" s="41"/>
+      <c r="D75" s="38"/>
+      <c r="E75" s="14" t="s">
+        <v>195</v>
+      </c>
       <c r="F75" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="G75" s="14" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="76" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D76" s="25"/>
-      <c r="E76" s="22"/>
+    <row r="76" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C76" s="42"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="14" t="s">
+        <v>186</v>
+      </c>
       <c r="F76" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="G76" s="14" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="77" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D77" s="20" t="s">
+    <row r="77" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C77" s="37" t="s">
         <v>187</v>
       </c>
-      <c r="E77" s="20" t="s">
+      <c r="D77" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="F77" s="16" t="s">
+      <c r="E77" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="G77" s="14" t="s">
+      <c r="F77" s="14" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="78" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D78" s="21"/>
-      <c r="E78" s="21"/>
-      <c r="F78" s="16" t="s">
+    <row r="78" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C78" s="38"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="16" t="s">
         <v>212</v>
       </c>
-      <c r="G78" s="13" t="s">
+      <c r="F78" s="13" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
-      <c r="F79" s="16" t="s">
+    <row r="79" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C79" s="38"/>
+      <c r="D79" s="38"/>
+      <c r="E79" s="16" t="s">
         <v>213</v>
       </c>
-      <c r="G79" s="13" t="s">
+      <c r="F79" s="13" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D80" s="21"/>
-      <c r="E80" s="21"/>
-      <c r="F80" s="16" t="s">
+    <row r="80" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C80" s="38"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="16" t="s">
         <v>214</v>
       </c>
-      <c r="G80" s="13" t="s">
+      <c r="F80" s="13" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="81" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D81" s="22"/>
-      <c r="E81" s="22"/>
-      <c r="F81" s="16" t="s">
+    <row r="81" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C81" s="39"/>
+      <c r="D81" s="39"/>
+      <c r="E81" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="G81" s="13" t="s">
+      <c r="F81" s="13" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="82" spans="4:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="D82" s="12" t="s">
+    <row r="82" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C82" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="E82" s="12"/>
-      <c r="F82" s="13" t="s">
+      <c r="D82" s="12"/>
+      <c r="E82" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="G82" s="14" t="s">
+      <c r="F82" s="14" t="s">
         <v>190</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="E68:E72"/>
-    <mergeCell ref="D73:G73"/>
-    <mergeCell ref="D52:G52"/>
-    <mergeCell ref="E53:E58"/>
-    <mergeCell ref="E42:E45"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="E59:E61"/>
-    <mergeCell ref="E62:E64"/>
-    <mergeCell ref="E46:E48"/>
-    <mergeCell ref="D49:G49"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="D31:G31"/>
-    <mergeCell ref="D38:G38"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E17:E22"/>
-    <mergeCell ref="E23:E26"/>
-    <mergeCell ref="E32:E34"/>
-    <mergeCell ref="E35:E37"/>
-    <mergeCell ref="D6:G6"/>
-    <mergeCell ref="D7:G7"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="D16:G16"/>
+    <mergeCell ref="D77:D81"/>
+    <mergeCell ref="C77:C81"/>
+    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="C74:C76"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="D39:D41"/>
     <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="D59:D61"/>
+    <mergeCell ref="D62:D64"/>
+    <mergeCell ref="D46:D48"/>
+    <mergeCell ref="C49:F49"/>
+    <mergeCell ref="D27:D30"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C38:F38"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D37"/>
+    <mergeCell ref="D65:D67"/>
     <mergeCell ref="D68:D72"/>
-    <mergeCell ref="E77:E81"/>
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="E74:E76"/>
-    <mergeCell ref="D74:D76"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="C52:F52"/>
+    <mergeCell ref="D53:D58"/>
+    <mergeCell ref="C68:C72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Document]_Update List UC và tiến độ dự án
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/List of UseCase.xlsx
+++ b/WIP/Users/HuyenPT/List of UseCase.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" refMode="R1C1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -537,18 +537,6 @@
     <t>Xóa nhà xuất bản</t>
   </si>
   <si>
-    <t>SYSTEM MODULE</t>
-  </si>
-  <si>
-    <t>Send confirm mail to active an account</t>
-  </si>
-  <si>
-    <t>Gửi mail xác nhận khi người dùng yêu cầu lập tài khoản</t>
-  </si>
-  <si>
-    <t>Gửi mail thông báo mật khẩu mới khi người dùng sử dụng chức năng quên mật khẩu</t>
-  </si>
-  <si>
     <t>UC050</t>
   </si>
   <si>
@@ -561,12 +549,6 @@
     <t>UC053</t>
   </si>
   <si>
-    <t>Statistic access times</t>
-  </si>
-  <si>
-    <t>Statistic</t>
-  </si>
-  <si>
     <t>Decline  request about reporting an account/group</t>
   </si>
   <si>
@@ -576,18 +558,12 @@
     <t>Suggest book/author</t>
   </si>
   <si>
-    <t>Send warning mail to reported user</t>
-  </si>
-  <si>
     <t>UC054</t>
   </si>
   <si>
     <t>UC055</t>
   </si>
   <si>
-    <t>Gửi mail cảnh cáo cho người dùng bị report</t>
-  </si>
-  <si>
     <t>Giới thiệu sách/tác giả cho người dùng: Dựa trên danh sách những sách họ bình chọn, tác giả đang theo dõi</t>
   </si>
   <si>
@@ -603,9 +579,6 @@
     <t>Delete publisher</t>
   </si>
   <si>
-    <t>Send  mail to reset password</t>
-  </si>
-  <si>
     <t>Reset pasword</t>
   </si>
   <si>
@@ -651,41 +624,26 @@
     <t>Xem thông tin thống kê lượt truy cập</t>
   </si>
   <si>
-    <t>Statistic users</t>
-  </si>
-  <si>
-    <t>Statistic authors</t>
-  </si>
-  <si>
-    <t>Statistic groups</t>
-  </si>
-  <si>
-    <t>Statistic books</t>
-  </si>
-  <si>
-    <t>Thống kê về người dùng thường</t>
-  </si>
-  <si>
-    <t>Thống kê về tác giả</t>
-  </si>
-  <si>
-    <t>Thống kê về nhóm</t>
-  </si>
-  <si>
-    <t>Thống kê về sách</t>
-  </si>
-  <si>
-    <t>Thống kê về lượt truy cập</t>
-  </si>
-  <si>
-    <t>Send mail</t>
+    <t>Show slides</t>
+  </si>
+  <si>
+    <t>Hiển thị các slide trên trang giới thiệu</t>
+  </si>
+  <si>
+    <t>Edit index of slides</t>
+  </si>
+  <si>
+    <t>Thay đổi thứ tự hiển thị slider ảnh trên trang giới thiệu</t>
+  </si>
+  <si>
+    <t>UC056</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -708,16 +666,8 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -739,12 +689,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -850,7 +794,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -885,20 +829,41 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -909,27 +874,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -947,36 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1279,7 +1193,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:F82"/>
+  <dimension ref="C5:F109"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
@@ -1307,27 +1221,27 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="24" t="s">
-        <v>198</v>
+      <c r="D8" s="15" t="s">
+        <v>189</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>6</v>
@@ -1337,8 +1251,8 @@
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1347,8 +1261,8 @@
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="26"/>
-      <c r="D10" s="25"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="16"/>
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1360,7 +1274,7 @@
       <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="26"/>
+      <c r="D11" s="17"/>
       <c r="E11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1369,10 +1283,10 @@
       </c>
     </row>
     <row r="12" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="D12" s="15" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1383,8 +1297,10 @@
       </c>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
+      <c r="C13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="17"/>
       <c r="E13" s="4" t="s">
         <v>131</v>
       </c>
@@ -1393,8 +1309,8 @@
       </c>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C14" s="5" t="s">
-        <v>20</v>
+      <c r="C14" s="4" t="s">
+        <v>22</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="4" t="s">
@@ -1405,30 +1321,30 @@
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C15" s="5" t="s">
-        <v>22</v>
+      <c r="C15" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="D15" s="5"/>
       <c r="E15" s="4" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="36"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="24" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1439,10 +1355,10 @@
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="D18" s="25"/>
+      <c r="C18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="16"/>
       <c r="E18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1451,8 +1367,8 @@
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="26"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="16"/>
       <c r="E19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1462,9 +1378,9 @@
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="25"/>
+        <v>36</v>
+      </c>
+      <c r="D20" s="16"/>
       <c r="E20" s="4" t="s">
         <v>31</v>
       </c>
@@ -1474,9 +1390,9 @@
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D21" s="25"/>
+        <v>37</v>
+      </c>
+      <c r="D21" s="16"/>
       <c r="E21" s="4" t="s">
         <v>53</v>
       </c>
@@ -1486,9 +1402,9 @@
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C22" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D22" s="26"/>
+        <v>38</v>
+      </c>
+      <c r="D22" s="17"/>
       <c r="E22" s="4" t="s">
         <v>54</v>
       </c>
@@ -1498,9 +1414,9 @@
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C23" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D23" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1512,9 +1428,9 @@
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C24" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D24" s="25"/>
+        <v>40</v>
+      </c>
+      <c r="D24" s="16"/>
       <c r="E24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1524,9 +1440,9 @@
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C25" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D25" s="25"/>
+        <v>41</v>
+      </c>
+      <c r="D25" s="16"/>
       <c r="E25" s="4" t="s">
         <v>43</v>
       </c>
@@ -1536,9 +1452,9 @@
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C26" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" s="26"/>
+        <v>49</v>
+      </c>
+      <c r="D26" s="17"/>
       <c r="E26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1546,9 +1462,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D27" s="21" t="s">
         <v>46</v>
@@ -1562,7 +1478,7 @@
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C28" s="5" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="D28" s="22"/>
       <c r="E28" s="4" t="s">
@@ -1574,7 +1490,7 @@
     </row>
     <row r="29" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C29" s="5" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="D29" s="22"/>
       <c r="E29" s="4" t="s">
@@ -1586,7 +1502,7 @@
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C30" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="D30" s="23"/>
       <c r="E30" s="4" t="s">
@@ -1604,12 +1520,12 @@
       <c r="E31" s="31"/>
       <c r="F31" s="32"/>
     </row>
-    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="15" t="s">
-        <v>73</v>
+    <row r="32" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="12" t="s">
+        <v>74</v>
       </c>
       <c r="D32" s="21" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>65</v>
@@ -1619,8 +1535,8 @@
       </c>
     </row>
     <row r="33" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C33" s="15" t="s">
-        <v>74</v>
+      <c r="C33" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="D33" s="22"/>
       <c r="E33" s="6" t="s">
@@ -1631,8 +1547,8 @@
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C34" s="15" t="s">
-        <v>81</v>
+      <c r="C34" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="D34" s="23"/>
       <c r="E34" s="6" t="s">
@@ -1643,11 +1559,11 @@
       </c>
     </row>
     <row r="35" spans="3:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C35" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" s="24" t="s">
-        <v>200</v>
+      <c r="C35" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>191</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>99</v>
@@ -1657,10 +1573,10 @@
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C36" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D36" s="25"/>
+      <c r="C36" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="D36" s="16"/>
       <c r="E36" s="4" t="s">
         <v>100</v>
       </c>
@@ -1669,10 +1585,10 @@
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C37" s="15" t="s">
-        <v>103</v>
-      </c>
-      <c r="D37" s="26"/>
+      <c r="C37" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D37" s="17"/>
       <c r="E37" s="4" t="s">
         <v>116</v>
       </c>
@@ -1690,10 +1606,10 @@
     </row>
     <row r="39" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C39" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="D39" s="24" t="s">
-        <v>201</v>
+        <v>105</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>192</v>
       </c>
       <c r="E39" s="4" t="s">
         <v>72</v>
@@ -1704,9 +1620,9 @@
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C40" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D40" s="25"/>
+        <v>106</v>
+      </c>
+      <c r="D40" s="16"/>
       <c r="E40" s="4" t="s">
         <v>84</v>
       </c>
@@ -1716,9 +1632,9 @@
     </row>
     <row r="41" spans="3:6" ht="60" x14ac:dyDescent="0.25">
       <c r="C41" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="26"/>
+        <v>107</v>
+      </c>
+      <c r="D41" s="17"/>
       <c r="E41" s="4" t="s">
         <v>88</v>
       </c>
@@ -1728,7 +1644,7 @@
     </row>
     <row r="42" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C42" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D42" s="21" t="s">
         <v>119</v>
@@ -1742,7 +1658,7 @@
     </row>
     <row r="43" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="D43" s="22"/>
       <c r="E43" s="6" t="s">
@@ -1754,7 +1670,7 @@
     </row>
     <row r="44" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D44" s="22"/>
       <c r="E44" s="4" t="s">
@@ -1766,7 +1682,7 @@
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D45" s="23"/>
       <c r="E45" s="4" t="s">
@@ -1778,9 +1694,9 @@
     </row>
     <row r="46" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C46" s="5" t="s">
-        <v>120</v>
-      </c>
-      <c r="D46" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="D46" s="15" t="s">
         <v>90</v>
       </c>
       <c r="E46" s="8" t="s">
@@ -1792,9 +1708,9 @@
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C47" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="D47" s="25"/>
+        <v>148</v>
+      </c>
+      <c r="D47" s="16"/>
       <c r="E47" s="4" t="s">
         <v>91</v>
       </c>
@@ -1804,9 +1720,9 @@
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C48" s="5" t="s">
-        <v>148</v>
-      </c>
-      <c r="D48" s="26"/>
+        <v>149</v>
+      </c>
+      <c r="D48" s="17"/>
       <c r="E48" s="4" t="s">
         <v>92</v>
       </c>
@@ -1824,7 +1740,7 @@
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="5" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D50" s="5"/>
       <c r="E50" s="4" t="s">
@@ -1836,7 +1752,7 @@
     </row>
     <row r="51" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C51" s="5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="D51" s="5"/>
       <c r="E51" s="6" t="s">
@@ -1846,380 +1762,503 @@
         <v>122</v>
       </c>
     </row>
-    <row r="52" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C52" s="20" t="s">
+    <row r="52" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C52" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" s="5"/>
+      <c r="E52" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C53" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="D52" s="20"/>
-      <c r="E52" s="20"/>
-      <c r="F52" s="20"/>
-    </row>
-    <row r="53" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C53" s="9" t="s">
-        <v>151</v>
-      </c>
-      <c r="D53" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="E53" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F53" s="10"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C54" s="9" t="s">
-        <v>152</v>
-      </c>
-      <c r="D54" s="18"/>
+        <v>153</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>123</v>
+      </c>
       <c r="E54" s="10" t="s">
-        <v>125</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>127</v>
-      </c>
+        <v>124</v>
+      </c>
+      <c r="F54" s="10"/>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C55" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="D55" s="18"/>
+        <v>154</v>
+      </c>
+      <c r="D55" s="25"/>
       <c r="E55" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F55" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C56" s="9" t="s">
-        <v>154</v>
-      </c>
-      <c r="D56" s="18"/>
+        <v>155</v>
+      </c>
+      <c r="D56" s="25"/>
       <c r="E56" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C57" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="D57" s="25"/>
+      <c r="E57" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="F56" s="10" t="s">
+      <c r="F57" s="10" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="57" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C57" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D57" s="18"/>
-      <c r="E57" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="F57" s="10" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="58" spans="3:6" ht="30" x14ac:dyDescent="0.25">
       <c r="C58" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D58" s="19"/>
+        <v>157</v>
+      </c>
+      <c r="D58" s="25"/>
       <c r="E58" s="11" t="s">
-        <v>184</v>
-      </c>
-      <c r="F58" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="F58" s="10" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="59" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C59" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D59" s="26"/>
+      <c r="E59" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F59" s="11" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C59" s="9" t="s">
-        <v>157</v>
-      </c>
-      <c r="D59" s="17" t="s">
-        <v>137</v>
-      </c>
-      <c r="E59" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F59" s="10" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C60" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D60" s="18"/>
+        <v>165</v>
+      </c>
+      <c r="D60" s="24" t="s">
+        <v>137</v>
+      </c>
       <c r="E60" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="61" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C61" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="D61" s="25"/>
+      <c r="E61" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="F60" s="10" t="s">
+      <c r="F61" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="61" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C61" s="9" t="s">
-        <v>165</v>
-      </c>
-      <c r="D61" s="19"/>
-      <c r="E61" s="11" t="s">
+    <row r="62" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C62" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="D62" s="26"/>
+      <c r="E62" s="11" t="s">
         <v>140</v>
       </c>
-      <c r="F61" s="10" t="s">
+      <c r="F62" s="10" t="s">
         <v>143</v>
-      </c>
-    </row>
-    <row r="62" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C62" s="9" t="s">
-        <v>166</v>
-      </c>
-      <c r="D62" s="17" t="s">
-        <v>144</v>
-      </c>
-      <c r="E62" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="F62" s="10" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C63" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="D63" s="18"/>
+        <v>168</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>144</v>
+      </c>
       <c r="E63" s="10" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="F63" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C64" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="D64" s="19"/>
+        <v>169</v>
+      </c>
+      <c r="D64" s="25"/>
       <c r="E64" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F64" s="10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C65" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="D65" s="17" t="s">
-        <v>191</v>
-      </c>
+        <v>173</v>
+      </c>
+      <c r="D65" s="25"/>
       <c r="E65" s="10" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C66" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D66" s="18"/>
+        <v>174</v>
+      </c>
+      <c r="D66" s="25"/>
       <c r="E66" s="10" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>171</v>
+        <v>203</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C67" s="9" t="s">
-        <v>178</v>
-      </c>
-      <c r="D67" s="19"/>
+        <v>175</v>
+      </c>
+      <c r="D67" s="26"/>
       <c r="E67" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F67" s="10" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="68" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C68" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="D68" s="24" t="s">
+        <v>183</v>
+      </c>
+      <c r="E68" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F68" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="69" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C69" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D69" s="25"/>
+      <c r="E69" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F69" s="10" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="70" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C70" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D70" s="26"/>
+      <c r="E70" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="71" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C71" s="24" t="s">
+        <v>206</v>
+      </c>
+      <c r="D71" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="E71" s="11" t="s">
         <v>194</v>
       </c>
-      <c r="F67" s="10" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="68" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C68" s="17" t="s">
-        <v>179</v>
-      </c>
-      <c r="D68" s="17" t="s">
-        <v>163</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="69" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C69" s="18"/>
-      <c r="D69" s="18"/>
-      <c r="E69" s="11" t="s">
-        <v>202</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="70" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C70" s="18"/>
-      <c r="D70" s="18"/>
-      <c r="E70" s="11" t="s">
-        <v>204</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="71" spans="3:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C71" s="18"/>
-      <c r="D71" s="18"/>
-      <c r="E71" s="11" t="s">
-        <v>205</v>
-      </c>
       <c r="F71" s="11" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="72" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C72" s="19"/>
-      <c r="D72" s="19"/>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="72" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
       <c r="E72" s="11" t="s">
+        <v>193</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="73" spans="3:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C73" s="25"/>
+      <c r="D73" s="25"/>
+      <c r="E73" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="74" spans="3:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C74" s="25"/>
+      <c r="D74" s="25"/>
+      <c r="E74" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" spans="3:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C75" s="26"/>
+      <c r="D75" s="26"/>
+      <c r="E75" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="F72" s="10" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="73" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C73" s="20" t="s">
-        <v>173</v>
-      </c>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20"/>
-      <c r="F73" s="20"/>
-    </row>
-    <row r="74" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C74" s="40" t="s">
-        <v>180</v>
-      </c>
-      <c r="D74" s="37" t="s">
-        <v>220</v>
-      </c>
-      <c r="E74" s="14" t="s">
-        <v>174</v>
-      </c>
-      <c r="F74" s="14" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="75" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C75" s="41"/>
-      <c r="D75" s="38"/>
-      <c r="E75" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="F75" s="14" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="76" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C76" s="42"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="F76" s="14" t="s">
-        <v>189</v>
-      </c>
+      <c r="F75" s="10" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="76" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C76"/>
+      <c r="D76"/>
+      <c r="E76"/>
+      <c r="F76"/>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C77" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="D77" s="37" t="s">
-        <v>182</v>
-      </c>
-      <c r="E77" s="16" t="s">
-        <v>211</v>
-      </c>
-      <c r="F77" s="14" t="s">
-        <v>215</v>
-      </c>
+      <c r="C77"/>
+      <c r="D77"/>
+      <c r="E77"/>
+      <c r="F77"/>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C78" s="38"/>
-      <c r="D78" s="38"/>
-      <c r="E78" s="16" t="s">
-        <v>212</v>
-      </c>
-      <c r="F78" s="13" t="s">
-        <v>216</v>
-      </c>
+      <c r="C78"/>
+      <c r="D78"/>
+      <c r="E78"/>
+      <c r="F78"/>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C79" s="38"/>
-      <c r="D79" s="38"/>
-      <c r="E79" s="16" t="s">
-        <v>213</v>
-      </c>
-      <c r="F79" s="13" t="s">
-        <v>217</v>
-      </c>
+      <c r="C79"/>
+      <c r="D79"/>
+      <c r="E79"/>
+      <c r="F79"/>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C80" s="38"/>
-      <c r="D80" s="38"/>
-      <c r="E80" s="16" t="s">
-        <v>214</v>
-      </c>
-      <c r="F80" s="13" t="s">
-        <v>218</v>
-      </c>
+      <c r="C80"/>
+      <c r="D80"/>
+      <c r="E80"/>
+      <c r="F80"/>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C81" s="39"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="16" t="s">
-        <v>181</v>
-      </c>
-      <c r="F81" s="13" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="82" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C82" s="12" t="s">
-        <v>188</v>
-      </c>
-      <c r="D82" s="12"/>
-      <c r="E82" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="F82" s="14" t="s">
-        <v>190</v>
-      </c>
+      <c r="C81"/>
+      <c r="D81"/>
+      <c r="E81"/>
+      <c r="F81"/>
+    </row>
+    <row r="82" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C82"/>
+      <c r="D82"/>
+      <c r="E82"/>
+      <c r="F82"/>
+    </row>
+    <row r="83" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C83"/>
+      <c r="D83"/>
+      <c r="E83"/>
+      <c r="F83"/>
+    </row>
+    <row r="84" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C84"/>
+      <c r="D84"/>
+      <c r="E84"/>
+      <c r="F84"/>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C85"/>
+      <c r="D85"/>
+      <c r="E85"/>
+      <c r="F85"/>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C86"/>
+      <c r="D86"/>
+      <c r="E86"/>
+      <c r="F86"/>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C87"/>
+      <c r="D87"/>
+      <c r="E87"/>
+      <c r="F87"/>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C88"/>
+      <c r="D88"/>
+      <c r="E88"/>
+      <c r="F88"/>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C89"/>
+      <c r="D89"/>
+      <c r="E89"/>
+      <c r="F89"/>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C90"/>
+      <c r="D90"/>
+      <c r="E90"/>
+      <c r="F90"/>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C91"/>
+      <c r="D91"/>
+      <c r="E91"/>
+      <c r="F91"/>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C92"/>
+      <c r="D92"/>
+      <c r="E92"/>
+      <c r="F92"/>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C93"/>
+      <c r="D93"/>
+      <c r="E93"/>
+      <c r="F93"/>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C94"/>
+      <c r="D94"/>
+      <c r="E94"/>
+      <c r="F94"/>
+    </row>
+    <row r="95" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C95"/>
+      <c r="D95"/>
+      <c r="E95"/>
+      <c r="F95"/>
+    </row>
+    <row r="96" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C96"/>
+      <c r="D96"/>
+      <c r="E96"/>
+      <c r="F96"/>
+    </row>
+    <row r="97" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C97"/>
+      <c r="D97"/>
+      <c r="E97"/>
+      <c r="F97"/>
+    </row>
+    <row r="98" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C98"/>
+      <c r="D98"/>
+      <c r="E98"/>
+      <c r="F98"/>
+    </row>
+    <row r="99" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C99"/>
+      <c r="D99"/>
+      <c r="E99"/>
+      <c r="F99"/>
+    </row>
+    <row r="100" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C100"/>
+      <c r="D100"/>
+      <c r="E100"/>
+      <c r="F100"/>
+    </row>
+    <row r="101" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C101"/>
+      <c r="D101"/>
+      <c r="E101"/>
+      <c r="F101"/>
+    </row>
+    <row r="102" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C102"/>
+      <c r="D102"/>
+      <c r="E102"/>
+      <c r="F102"/>
+    </row>
+    <row r="103" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C103"/>
+      <c r="D103"/>
+      <c r="E103"/>
+      <c r="F103"/>
+    </row>
+    <row r="104" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C104"/>
+      <c r="D104"/>
+      <c r="E104"/>
+      <c r="F104"/>
+    </row>
+    <row r="105" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C105"/>
+      <c r="D105"/>
+      <c r="E105"/>
+      <c r="F105"/>
+    </row>
+    <row r="106" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C106"/>
+      <c r="D106"/>
+      <c r="E106"/>
+      <c r="F106"/>
+    </row>
+    <row r="107" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C107"/>
+      <c r="D107"/>
+      <c r="E107"/>
+      <c r="F107"/>
+    </row>
+    <row r="108" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C108"/>
+      <c r="D108"/>
+      <c r="E108"/>
+      <c r="F108"/>
+    </row>
+    <row r="109" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C109"/>
+      <c r="D109"/>
+      <c r="E109"/>
+      <c r="F109"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="D77:D81"/>
-    <mergeCell ref="C77:C81"/>
-    <mergeCell ref="D74:D76"/>
-    <mergeCell ref="C74:C76"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="D42:D45"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="D59:D61"/>
-    <mergeCell ref="D62:D64"/>
-    <mergeCell ref="D46:D48"/>
+  <mergeCells count="25">
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="D63:D67"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="C71:C75"/>
+    <mergeCell ref="D71:D75"/>
     <mergeCell ref="C49:F49"/>
     <mergeCell ref="D27:D30"/>
     <mergeCell ref="C31:F31"/>
@@ -2229,12 +2268,15 @@
     <mergeCell ref="D23:D26"/>
     <mergeCell ref="D32:D34"/>
     <mergeCell ref="D35:D37"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="D68:D72"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="C52:F52"/>
-    <mergeCell ref="D53:D58"/>
-    <mergeCell ref="C68:C72"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D42:D45"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="D46:D48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Doc]_Cập nhập tiến độ dự án và commit meeting minute
Mọi người đọc kỹ Meeting Minute để tránh miss task nhé
</commit_message>
<xml_diff>
--- a/WIP/Users/HuyenPT/List of UseCase.xlsx
+++ b/WIP/Users/HuyenPT/List of UseCase.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="214">
   <si>
     <t>Use Case No.</t>
   </si>
@@ -637,6 +637,27 @@
   </si>
   <si>
     <t>UC056</t>
+  </si>
+  <si>
+    <t>UC057</t>
+  </si>
+  <si>
+    <t>Manage Group</t>
+  </si>
+  <si>
+    <t>Band a group</t>
+  </si>
+  <si>
+    <t>cấm 1 nhóm</t>
+  </si>
+  <si>
+    <t>UC058</t>
+  </si>
+  <si>
+    <t>Unban a group</t>
+  </si>
+  <si>
+    <t>gỡ bỏ lệnh cấm nhóm</t>
   </si>
 </sst>
 </file>
@@ -794,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -835,18 +856,54 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -856,41 +913,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1229,18 +1253,18 @@
       <c r="F6" s="13"/>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="26" t="s">
         <v>189</v>
       </c>
       <c r="E8" s="4" t="s">
@@ -1251,8 +1275,8 @@
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
       <c r="E9" s="4" t="s">
         <v>7</v>
       </c>
@@ -1261,8 +1285,8 @@
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="17"/>
-      <c r="D10" s="16"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="28"/>
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1274,7 +1298,7 @@
       <c r="C11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="17"/>
+      <c r="D11" s="27"/>
       <c r="E11" s="4" t="s">
         <v>13</v>
       </c>
@@ -1286,7 +1310,7 @@
       <c r="C12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="15" t="s">
+      <c r="D12" s="26" t="s">
         <v>17</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1300,7 +1324,7 @@
       <c r="C13" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="4" t="s">
         <v>131</v>
       </c>
@@ -1333,18 +1357,18 @@
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="D16" s="19"/>
-      <c r="E16" s="19"/>
-      <c r="F16" s="20"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C17" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="26" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -1355,10 +1379,10 @@
       </c>
     </row>
     <row r="18" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="16"/>
+      <c r="D18" s="28"/>
       <c r="E18" s="4" t="s">
         <v>27</v>
       </c>
@@ -1367,8 +1391,8 @@
       </c>
     </row>
     <row r="19" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C19" s="17"/>
-      <c r="D19" s="16"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="28"/>
       <c r="E19" s="4" t="s">
         <v>28</v>
       </c>
@@ -1380,7 +1404,7 @@
       <c r="C20" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D20" s="16"/>
+      <c r="D20" s="28"/>
       <c r="E20" s="4" t="s">
         <v>31</v>
       </c>
@@ -1392,7 +1416,7 @@
       <c r="C21" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D21" s="16"/>
+      <c r="D21" s="28"/>
       <c r="E21" s="4" t="s">
         <v>53</v>
       </c>
@@ -1404,7 +1428,7 @@
       <c r="C22" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D22" s="17"/>
+      <c r="D22" s="27"/>
       <c r="E22" s="4" t="s">
         <v>54</v>
       </c>
@@ -1416,7 +1440,7 @@
       <c r="C23" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="26" t="s">
         <v>48</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -1430,7 +1454,7 @@
       <c r="C24" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="16"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1442,7 +1466,7 @@
       <c r="C25" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="16"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="4" t="s">
         <v>43</v>
       </c>
@@ -1454,7 +1478,7 @@
       <c r="C26" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D26" s="17"/>
+      <c r="D26" s="27"/>
       <c r="E26" s="4" t="s">
         <v>34</v>
       </c>
@@ -1466,7 +1490,7 @@
       <c r="C27" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="20" t="s">
         <v>46</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -1480,7 +1504,7 @@
       <c r="C28" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="22"/>
+      <c r="D28" s="21"/>
       <c r="E28" s="4" t="s">
         <v>44</v>
       </c>
@@ -1492,7 +1516,7 @@
       <c r="C29" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="D29" s="22"/>
+      <c r="D29" s="21"/>
       <c r="E29" s="4" t="s">
         <v>45</v>
       </c>
@@ -1504,7 +1528,7 @@
       <c r="C30" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="D30" s="23"/>
+      <c r="D30" s="22"/>
       <c r="E30" s="4" t="s">
         <v>35</v>
       </c>
@@ -1513,18 +1537,18 @@
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="32"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="25"/>
     </row>
     <row r="32" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="20" t="s">
         <v>190</v>
       </c>
       <c r="E32" s="4" t="s">
@@ -1538,7 +1562,7 @@
       <c r="C33" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="D33" s="22"/>
+      <c r="D33" s="21"/>
       <c r="E33" s="6" t="s">
         <v>69</v>
       </c>
@@ -1550,7 +1574,7 @@
       <c r="C34" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="D34" s="23"/>
+      <c r="D34" s="22"/>
       <c r="E34" s="6" t="s">
         <v>115</v>
       </c>
@@ -1562,7 +1586,7 @@
       <c r="C35" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="26" t="s">
         <v>191</v>
       </c>
       <c r="E35" s="4" t="s">
@@ -1576,7 +1600,7 @@
       <c r="C36" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="D36" s="16"/>
+      <c r="D36" s="28"/>
       <c r="E36" s="4" t="s">
         <v>100</v>
       </c>
@@ -1588,7 +1612,7 @@
       <c r="C37" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="D37" s="17"/>
+      <c r="D37" s="27"/>
       <c r="E37" s="4" t="s">
         <v>116</v>
       </c>
@@ -1597,18 +1621,18 @@
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="29"/>
+      <c r="D38" s="18"/>
+      <c r="E38" s="18"/>
+      <c r="F38" s="19"/>
     </row>
     <row r="39" spans="3:6" ht="45" x14ac:dyDescent="0.25">
       <c r="C39" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="26" t="s">
         <v>192</v>
       </c>
       <c r="E39" s="4" t="s">
@@ -1622,7 +1646,7 @@
       <c r="C40" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="D40" s="16"/>
+      <c r="D40" s="28"/>
       <c r="E40" s="4" t="s">
         <v>84</v>
       </c>
@@ -1634,7 +1658,7 @@
       <c r="C41" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="17"/>
+      <c r="D41" s="27"/>
       <c r="E41" s="4" t="s">
         <v>88</v>
       </c>
@@ -1646,7 +1670,7 @@
       <c r="C42" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="20" t="s">
         <v>119</v>
       </c>
       <c r="E42" s="6" t="s">
@@ -1660,7 +1684,7 @@
       <c r="C43" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="D43" s="22"/>
+      <c r="D43" s="21"/>
       <c r="E43" s="6" t="s">
         <v>76</v>
       </c>
@@ -1672,7 +1696,7 @@
       <c r="C44" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="D44" s="22"/>
+      <c r="D44" s="21"/>
       <c r="E44" s="4" t="s">
         <v>77</v>
       </c>
@@ -1684,7 +1708,7 @@
       <c r="C45" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D45" s="23"/>
+      <c r="D45" s="22"/>
       <c r="E45" s="4" t="s">
         <v>82</v>
       </c>
@@ -1696,7 +1720,7 @@
       <c r="C46" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="26" t="s">
         <v>90</v>
       </c>
       <c r="E46" s="8" t="s">
@@ -1710,7 +1734,7 @@
       <c r="C47" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="D47" s="16"/>
+      <c r="D47" s="28"/>
       <c r="E47" s="4" t="s">
         <v>91</v>
       </c>
@@ -1722,7 +1746,7 @@
       <c r="C48" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="D48" s="17"/>
+      <c r="D48" s="27"/>
       <c r="E48" s="4" t="s">
         <v>92</v>
       </c>
@@ -1731,12 +1755,12 @@
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="D49" s="28"/>
-      <c r="E49" s="28"/>
-      <c r="F49" s="29"/>
+      <c r="D49" s="18"/>
+      <c r="E49" s="18"/>
+      <c r="F49" s="19"/>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C50" s="5" t="s">
@@ -1786,7 +1810,7 @@
       <c r="C54" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="D54" s="24" t="s">
+      <c r="D54" s="14" t="s">
         <v>123</v>
       </c>
       <c r="E54" s="10" t="s">
@@ -1798,7 +1822,7 @@
       <c r="C55" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="D55" s="25"/>
+      <c r="D55" s="15"/>
       <c r="E55" s="10" t="s">
         <v>125</v>
       </c>
@@ -1810,7 +1834,7 @@
       <c r="C56" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="D56" s="25"/>
+      <c r="D56" s="15"/>
       <c r="E56" s="10" t="s">
         <v>126</v>
       </c>
@@ -1822,7 +1846,7 @@
       <c r="C57" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="D57" s="25"/>
+      <c r="D57" s="15"/>
       <c r="E57" s="10" t="s">
         <v>129</v>
       </c>
@@ -1834,7 +1858,7 @@
       <c r="C58" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="D58" s="25"/>
+      <c r="D58" s="15"/>
       <c r="E58" s="11" t="s">
         <v>177</v>
       </c>
@@ -1846,7 +1870,7 @@
       <c r="C59" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D59" s="26"/>
+      <c r="D59" s="16"/>
       <c r="E59" s="11" t="s">
         <v>178</v>
       </c>
@@ -1858,7 +1882,7 @@
       <c r="C60" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="D60" s="24" t="s">
+      <c r="D60" s="14" t="s">
         <v>137</v>
       </c>
       <c r="E60" s="10" t="s">
@@ -1872,7 +1896,7 @@
       <c r="C61" s="9" t="s">
         <v>166</v>
       </c>
-      <c r="D61" s="25"/>
+      <c r="D61" s="15"/>
       <c r="E61" s="10" t="s">
         <v>139</v>
       </c>
@@ -1884,7 +1908,7 @@
       <c r="C62" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="D62" s="26"/>
+      <c r="D62" s="16"/>
       <c r="E62" s="11" t="s">
         <v>140</v>
       </c>
@@ -1896,7 +1920,7 @@
       <c r="C63" s="9" t="s">
         <v>168</v>
       </c>
-      <c r="D63" s="24" t="s">
+      <c r="D63" s="14" t="s">
         <v>144</v>
       </c>
       <c r="E63" s="10" t="s">
@@ -1910,7 +1934,7 @@
       <c r="C64" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="D64" s="25"/>
+      <c r="D64" s="15"/>
       <c r="E64" s="10" t="s">
         <v>145</v>
       </c>
@@ -1922,7 +1946,7 @@
       <c r="C65" s="9" t="s">
         <v>173</v>
       </c>
-      <c r="D65" s="25"/>
+      <c r="D65" s="15"/>
       <c r="E65" s="10" t="s">
         <v>146</v>
       </c>
@@ -1934,7 +1958,7 @@
       <c r="C66" s="9" t="s">
         <v>174</v>
       </c>
-      <c r="D66" s="25"/>
+      <c r="D66" s="15"/>
       <c r="E66" s="10" t="s">
         <v>202</v>
       </c>
@@ -1946,7 +1970,7 @@
       <c r="C67" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="D67" s="26"/>
+      <c r="D67" s="16"/>
       <c r="E67" s="10" t="s">
         <v>204</v>
       </c>
@@ -1958,7 +1982,7 @@
       <c r="C68" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="D68" s="24" t="s">
+      <c r="D68" s="14" t="s">
         <v>183</v>
       </c>
       <c r="E68" s="10" t="s">
@@ -1972,7 +1996,7 @@
       <c r="C69" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D69" s="25"/>
+      <c r="D69" s="15"/>
       <c r="E69" s="10" t="s">
         <v>185</v>
       </c>
@@ -1984,7 +2008,7 @@
       <c r="C70" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="D70" s="26"/>
+      <c r="D70" s="16"/>
       <c r="E70" s="10" t="s">
         <v>186</v>
       </c>
@@ -1993,10 +2017,10 @@
       </c>
     </row>
     <row r="71" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C71" s="24" t="s">
+      <c r="C71" s="14" t="s">
         <v>206</v>
       </c>
-      <c r="D71" s="24" t="s">
+      <c r="D71" s="14" t="s">
         <v>163</v>
       </c>
       <c r="E71" s="11" t="s">
@@ -2007,8 +2031,8 @@
       </c>
     </row>
     <row r="72" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C72" s="25"/>
-      <c r="D72" s="25"/>
+      <c r="C72" s="15"/>
+      <c r="D72" s="15"/>
       <c r="E72" s="11" t="s">
         <v>193</v>
       </c>
@@ -2017,8 +2041,8 @@
       </c>
     </row>
     <row r="73" spans="3:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="C73" s="25"/>
-      <c r="D73" s="25"/>
+      <c r="C73" s="15"/>
+      <c r="D73" s="15"/>
       <c r="E73" s="11" t="s">
         <v>195</v>
       </c>
@@ -2027,8 +2051,8 @@
       </c>
     </row>
     <row r="74" spans="3:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
+      <c r="C74" s="15"/>
+      <c r="D74" s="15"/>
       <c r="E74" s="11" t="s">
         <v>196</v>
       </c>
@@ -2037,8 +2061,8 @@
       </c>
     </row>
     <row r="75" spans="3:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="C75" s="26"/>
-      <c r="D75" s="26"/>
+      <c r="C75" s="16"/>
+      <c r="D75" s="16"/>
       <c r="E75" s="11" t="s">
         <v>164</v>
       </c>
@@ -2047,16 +2071,30 @@
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C76"/>
-      <c r="D76"/>
-      <c r="E76"/>
-      <c r="F76"/>
+      <c r="C76" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D76" s="33" t="s">
+        <v>208</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>209</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C77"/>
-      <c r="D77"/>
-      <c r="E77"/>
-      <c r="F77"/>
+      <c r="C77" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D77" s="33"/>
+      <c r="E77" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C78"/>
@@ -2251,32 +2289,33 @@
       <c r="F109"/>
     </row>
   </sheetData>
-  <mergeCells count="25">
-    <mergeCell ref="C53:F53"/>
-    <mergeCell ref="D54:D59"/>
-    <mergeCell ref="D60:D62"/>
-    <mergeCell ref="D63:D67"/>
-    <mergeCell ref="D68:D70"/>
+  <mergeCells count="26">
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:C10"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D17:D22"/>
+    <mergeCell ref="D23:D26"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="D35:D37"/>
     <mergeCell ref="C71:C75"/>
     <mergeCell ref="D71:D75"/>
     <mergeCell ref="C49:F49"/>
     <mergeCell ref="D27:D30"/>
     <mergeCell ref="C31:F31"/>
     <mergeCell ref="C38:F38"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D17:D22"/>
-    <mergeCell ref="D23:D26"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="D35:D37"/>
-    <mergeCell ref="C6:F6"/>
-    <mergeCell ref="C7:F7"/>
-    <mergeCell ref="C8:C10"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="D8:D11"/>
     <mergeCell ref="D42:D45"/>
     <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D12:D13"/>
     <mergeCell ref="D46:D48"/>
+    <mergeCell ref="C53:F53"/>
+    <mergeCell ref="D54:D59"/>
+    <mergeCell ref="D60:D62"/>
+    <mergeCell ref="D63:D67"/>
+    <mergeCell ref="D68:D70"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>